<commit_message>
Update 2018-10-03 23:04 UTC+08:00
</commit_message>
<xml_diff>
--- a/Word/LSOI2018 Preround 2nd/result.xlsx
+++ b/Word/LSOI2018 Preround 2nd/result.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">排名</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">曾卓轩</t>
   </si>
   <si>
+    <t xml:space="preserve">谢楠</t>
+  </si>
+  <si>
     <t xml:space="preserve">苏思哲</t>
   </si>
   <si>
@@ -58,29 +61,13 @@
     <t xml:space="preserve">邓涵</t>
   </si>
   <si>
-    <t xml:space="preserve">zyh</t>
+    <t xml:space="preserve">郑义航</t>
   </si>
   <si>
     <t xml:space="preserve">侯东杰</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK JP Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">20200234</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">答案</t>
-    </r>
+    <t xml:space="preserve">许婉婷</t>
   </si>
   <si>
     <t xml:space="preserve">林熙然</t>
@@ -235,10 +222,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -259,7 +246,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <f aca="false">RANK(B2,B$2:B$20)</f>
+        <f aca="false">RANK(B2,B$2:B$21)</f>
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
@@ -271,7 +258,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <f aca="false">RANK(B3,B$2:B$20)</f>
+        <f aca="false">RANK(B3,B$2:B$21)</f>
         <v>2</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -283,7 +270,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <f aca="false">RANK(B4,B$2:B$20)</f>
+        <f aca="false">RANK(B4,B$2:B$21)</f>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -295,7 +282,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <f aca="false">RANK(B5,B$2:B$20)</f>
+        <f aca="false">RANK(B5,B$2:B$21)</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -307,11 +294,11 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <f aca="false">RANK(B6,B$2:B$20)</f>
+        <f aca="false">RANK(B6,B$2:B$21)</f>
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>54</v>
+      <c r="B6" s="2" t="n">
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -319,11 +306,11 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <f aca="false">RANK(B7,B$2:B$20)</f>
+        <f aca="false">RANK(B7,B$2:B$21)</f>
         <v>6</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -331,11 +318,11 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <f aca="false">RANK(B8,B$2:B$20)</f>
+        <f aca="false">RANK(B8,B$2:B$21)</f>
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>45</v>
+      <c r="B8" s="4" t="n">
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -343,11 +330,11 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <f aca="false">RANK(B9,B$2:B$20)</f>
+        <f aca="false">RANK(B9,B$2:B$21)</f>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>42</v>
+      <c r="B9" s="2" t="n">
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
@@ -355,11 +342,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <f aca="false">RANK(B10,B$2:B$20)</f>
+        <f aca="false">RANK(B10,B$2:B$21)</f>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
@@ -367,23 +354,23 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <f aca="false">RANK(B11,B$2:B$20)</f>
+        <f aca="false">RANK(B11,B$2:B$21)</f>
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <f aca="false">RANK(B12,B$2:B$20)</f>
+        <f aca="false">RANK(B12,B$2:B$21)</f>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>13</v>
@@ -391,23 +378,23 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <f aca="false">RANK(B13,B$2:B$20)</f>
+        <f aca="false">RANK(B13,B$2:B$21)</f>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <f aca="false">RANK(B14,B$2:B$20)</f>
+        <f aca="false">RANK(B14,B$2:B$21)</f>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>15</v>
@@ -415,11 +402,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <f aca="false">RANK(B15,B$2:B$20)</f>
+        <f aca="false">RANK(B15,B$2:B$21)</f>
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>28</v>
+      <c r="B15" s="2" t="n">
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>16</v>
@@ -427,11 +414,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <f aca="false">RANK(B16,B$2:B$20)</f>
+        <f aca="false">RANK(B16,B$2:B$21)</f>
         <v>15</v>
       </c>
       <c r="B16" s="4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
@@ -439,11 +426,11 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <f aca="false">RANK(B17,B$2:B$20)</f>
+        <f aca="false">RANK(B17,B$2:B$21)</f>
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>20</v>
+      <c r="B17" s="4" t="n">
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>18</v>
@@ -451,10 +438,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <f aca="false">RANK(B18,B$2:B$20)</f>
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="n">
+        <f aca="false">RANK(B18,B$2:B$21)</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -463,26 +450,38 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <f aca="false">RANK(B19,B$2:B$20)</f>
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <f aca="false">RANK(B19,B$2:B$21)</f>
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <f aca="false">RANK(B20,B$2:B$20)</f>
-        <v>18</v>
+        <f aca="false">RANK(B20,B$2:B$21)</f>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <f aca="false">RANK(B21,B$2:B$21)</f>
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>